<commit_message>
. adding num lock support
</commit_message>
<xml_diff>
--- a/scan_codes.xlsx
+++ b/scan_codes.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="259">
   <si>
     <t>ESC</t>
   </si>
@@ -882,7 +882,77 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="15">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1332,8 +1402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE169"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A92" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7563,9 +7633,8 @@
       <c r="C99">
         <v>98</v>
       </c>
-      <c r="D99" t="e">
-        <f>VLOOKUP(C98,'PS2 Scancodes'!$B$3:$C$103,2,0)</f>
-        <v>#N/A</v>
+      <c r="D99" t="s">
+        <v>69</v>
       </c>
       <c r="E99">
         <v>60</v>
@@ -7576,11 +7645,11 @@
       </c>
       <c r="G99">
         <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="H99" t="e">
+        <v>92</v>
+      </c>
+      <c r="H99" t="str">
         <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>\</v>
       </c>
       <c r="I99">
         <v>62</v>
@@ -7589,9 +7658,12 @@
         <f t="shared" si="16"/>
         <v>&gt;</v>
       </c>
+      <c r="K99" t="s">
+        <v>133</v>
+      </c>
       <c r="L99">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="M99">
         <v>124</v>
@@ -8292,9 +8364,8 @@
       <c r="C111">
         <v>110</v>
       </c>
-      <c r="D111" t="e">
-        <f>VLOOKUP(C110,'PS2 Scancodes'!$B$3:$C$103,2,0)</f>
-        <v>#N/A</v>
+      <c r="D111" t="s">
+        <v>28</v>
       </c>
       <c r="E111">
         <v>0</v>
@@ -8305,11 +8376,11 @@
       </c>
       <c r="G111">
         <f>IF(ISERROR(CODE(D111)),0,CODE(D111))</f>
-        <v>0</v>
-      </c>
-      <c r="H111" t="e">
+        <v>46</v>
+      </c>
+      <c r="H111" t="str">
         <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>.</v>
       </c>
       <c r="I111">
         <v>0</v>
@@ -8487,11 +8558,11 @@
         <v>#VALUE!</v>
       </c>
       <c r="G114">
-        <v>0</v>
-      </c>
-      <c r="H114" t="e">
+        <v>48</v>
+      </c>
+      <c r="H114" t="str">
         <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>0</v>
       </c>
       <c r="I114">
         <v>0</v>
@@ -10341,27 +10412,27 @@
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:H129 G2">
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="14" priority="3">
       <formula>E2=G2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E129">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J129">
-    <cfRule type="expression" dxfId="2" priority="5">
+    <cfRule type="expression" dxfId="12" priority="5">
       <formula>F3=J3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S129">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="11" priority="1">
       <formula>S2=Q2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I129">
-    <cfRule type="expression" dxfId="0" priority="7">
+    <cfRule type="expression" dxfId="10" priority="7">
       <formula>F2=I2</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
. bit time fix in send command byte - it was causing problems with some keyboards
</commit_message>
<xml_diff>
--- a/scan_codes.xlsx
+++ b/scan_codes.xlsx
@@ -882,77 +882,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
@@ -1403,7 +1333,7 @@
   <dimension ref="A1:AE169"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A92" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L129"/>
+      <selection activeCell="Q2" sqref="Q2:Q129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7673,11 +7603,11 @@
         <v>|</v>
       </c>
       <c r="Q99">
-        <v>0</v>
-      </c>
-      <c r="R99" t="e">
+        <v>28</v>
+      </c>
+      <c r="R99" t="str">
         <f t="shared" si="11"/>
-        <v>#VALUE!</v>
+        <v>_x001C_</v>
       </c>
       <c r="S99">
         <f t="shared" si="19"/>
@@ -10412,27 +10342,27 @@
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:H129 G2">
-    <cfRule type="expression" dxfId="14" priority="3">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>E2=G2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E129">
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J129">
-    <cfRule type="expression" dxfId="12" priority="5">
+    <cfRule type="expression" dxfId="2" priority="5">
       <formula>F3=J3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S129">
-    <cfRule type="expression" dxfId="11" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>S2=Q2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I129">
-    <cfRule type="expression" dxfId="10" priority="7">
+    <cfRule type="expression" dxfId="0" priority="7">
       <formula>F2=I2</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>